<commit_message>
Assignment Rework - 08/05
</commit_message>
<xml_diff>
--- a/Rahul Assignment/assignment2/src/output.xlsx
+++ b/Rahul Assignment/assignment2/src/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Employee ID</t>
   </si>
@@ -23,34 +23,22 @@
     <t>Department</t>
   </si>
   <si>
-    <t>Dark</t>
+    <t>Rahul</t>
   </si>
   <si>
-    <t>Engg</t>
+    <t>QA</t>
   </si>
   <si>
-    <t>Happy</t>
+    <t>Nitin</t>
   </si>
   <si>
-    <t>Marketing</t>
+    <t>Binu</t>
   </si>
   <si>
-    <t>June</t>
+    <t>Dev</t>
   </si>
   <si>
-    <t>SEO</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>Inusrance</t>
-  </si>
-  <si>
-    <t>Mathew</t>
-  </si>
-  <si>
-    <t>Bussiness</t>
+    <t>joy</t>
   </si>
 </sst>
 </file>
@@ -95,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -131,7 +119,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -139,10 +127,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -150,21 +138,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>